<commit_message>
added version that takes in all 3 datatypes
</commit_message>
<xml_diff>
--- a/testDat/test_aneupl_4color_1.xlsx
+++ b/testDat/test_aneupl_4color_1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2180" windowWidth="27360" windowHeight="14220" tabRatio="500"/>
+    <workbookView xWindow="1920" yWindow="460" windowWidth="27360" windowHeight="14220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -376,8 +376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -398,7 +398,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -412,7 +412,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>4</v>

</xml_diff>